<commit_message>
Update & fix bug for VCCT1 on 2014.9.3
</commit_message>
<xml_diff>
--- a/beas_aplatz_resource_gene&sche_trp01.xlsx
+++ b/beas_aplatz_resource_gene&sche_trp01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15180" windowHeight="7815"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14220" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="79">
   <si>
     <t>Resource (String, 20)</t>
   </si>
@@ -54,24 +54,6 @@
     <t>Shift schedule resources (String, 20)</t>
   </si>
   <si>
-    <t>String, 20</t>
-  </si>
-  <si>
-    <t>String, 255</t>
-  </si>
-  <si>
-    <t>String, 30</t>
-  </si>
-  <si>
-    <t>String, J:Yes, N:No</t>
-  </si>
-  <si>
-    <t>Long, 1:Yes, 0:No</t>
-  </si>
-  <si>
-    <t>Number, (19,6)</t>
-  </si>
-  <si>
     <t>aplatz_id</t>
   </si>
   <si>
@@ -262,6 +244,15 @@
   </si>
   <si>
     <t>Store</t>
+  </si>
+  <si>
+    <t>S/N tag (String, Y:Yes, N:No)</t>
+  </si>
+  <si>
+    <t>p_serialnumtag</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -600,15 +591,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L25"/>
+      <selection sqref="A1:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -645,8 +639,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -657,72 +654,78 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
+        <v>28</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -730,215 +733,230 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7">
         <v>8</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5">
-        <v>24</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7">
-        <v>24</v>
       </c>
       <c r="K7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
       <c r="J8">
         <v>8</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -947,24 +965,27 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -973,74 +994,80 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J10">
+        <v>24</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11">
         <v>8</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11">
-        <v>24</v>
       </c>
       <c r="K11">
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1049,264 +1076,285 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J12">
         <v>8</v>
       </c>
       <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13">
+        <v>24</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13">
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>24</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16">
         <v>8</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14">
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17">
         <v>24</v>
       </c>
-      <c r="K14">
+      <c r="K17">
         <v>2</v>
       </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15">
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18">
         <v>8</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16">
-        <v>24</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18">
-        <v>24</v>
       </c>
       <c r="K18">
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1315,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J19">
         <v>8</v>
@@ -1327,24 +1375,27 @@
         <v>2</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1353,10 +1404,10 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J20">
         <v>8</v>
@@ -1365,24 +1416,27 @@
         <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1391,10 +1445,10 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J21">
         <v>8</v>
@@ -1403,24 +1457,27 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1429,36 +1486,39 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J22">
         <v>8</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1467,36 +1527,39 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J23">
         <v>8</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1505,57 +1568,22 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J24">
         <v>8</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25">
-        <v>8</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>